<commit_message>
ajout rhs ssr tests
</commit_message>
<xml_diff>
--- a/formats/regpexpr/rg_curseurs.xlsx
+++ b/formats/regpexpr/rg_curseurs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28016"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Github/formats_pmeasyr/formats/regpexpr/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="24240" windowHeight="12855"/>
+    <workbookView xWindow="1400" yWindow="460" windowWidth="27400" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,11 +17,19 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="29">
   <si>
     <t>table</t>
   </si>
@@ -88,19 +101,28 @@
   </si>
   <si>
     <t>.{1,29}</t>
+  </si>
+  <si>
+    <t>rhs</t>
+  </si>
+  <si>
+    <t>zcsarr</t>
+  </si>
+  <si>
+    <t>.{1,35}</t>
+  </si>
+  <si>
+    <t>.{1,23}</t>
+  </si>
+  <si>
+    <t>.{1,22}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,351 +139,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -469,309 +161,28 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
-    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="Title" xfId="40" builtinId="15"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -780,7 +191,7 @@
   <a:themeElements>
     <a:clrScheme name="Bureau">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="4C4C4C"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1061,20 +472,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:E61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="141" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58:B61"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="141" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1091,7 +501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1108,7 +518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1125,7 +535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1142,7 +552,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1159,7 +569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1176,7 +586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1193,7 +603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1210,7 +620,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1227,7 +637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1244,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1261,7 +671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1278,7 +688,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1295,7 +705,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1312,7 +722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1329,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1346,7 +756,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1363,7 +773,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1380,7 +790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1397,7 +807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1414,7 +824,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1431,7 +841,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1448,7 +858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1465,7 +875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1482,7 +892,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1499,7 +909,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1516,7 +926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1533,7 +943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1550,7 +960,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1567,7 +977,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1584,7 +994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1601,7 +1011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1618,7 +1028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1635,7 +1045,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1652,7 +1062,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1669,7 +1079,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1686,7 +1096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1703,7 +1113,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1720,7 +1130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -1737,7 +1147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -1754,7 +1164,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -1771,7 +1181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1788,7 +1198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -1805,7 +1215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1822,7 +1232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1839,7 +1249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1856,7 +1266,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1873,7 +1283,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1890,7 +1300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1907,7 +1317,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1924,7 +1334,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -1941,7 +1351,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -1958,7 +1368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -1975,7 +1385,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -1992,7 +1402,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -2009,7 +1419,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -2026,7 +1436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -2043,7 +1453,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>17</v>
       </c>
@@ -2060,7 +1470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>17</v>
       </c>
@@ -2077,7 +1487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>17</v>
       </c>
@@ -2094,7 +1504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>17</v>
       </c>
@@ -2111,40 +1521,133 @@
         <v>29</v>
       </c>
     </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="5">
+        <v>2016</v>
+      </c>
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="5">
+        <v>2016</v>
+      </c>
+      <c r="C63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" t="s">
+        <v>26</v>
+      </c>
+      <c r="E63">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" s="5">
+        <v>2016</v>
+      </c>
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" s="5">
+        <v>2015</v>
+      </c>
+      <c r="C65" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="5">
+        <v>2015</v>
+      </c>
+      <c r="C66" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="5">
+        <v>2015</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout curseurs regexpr parties variables pour 2019
</commit_message>
<xml_diff>
--- a/formats/regpexpr/rg_curseurs.xlsx
+++ b/formats/regpexpr/rg_curseurs.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Github/formats_pmeasyr/formats/regpexpr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/regpexpr/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F03274-5B65-004A-95CD-665993999529}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="27340" windowHeight="17540"/>
+    <workbookView xWindow="1460" yWindow="460" windowWidth="27340" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$E$75</definedName>
+  </definedNames>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="29">
   <si>
     <t>table</t>
   </si>
@@ -121,7 +125,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -181,6 +185,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -472,11 +479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="141" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72:B75"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="141" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76:B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1759,13 +1766,149 @@
         <v>24</v>
       </c>
     </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B76" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B77" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E77" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B78" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E78" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B79" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="1">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1777,7 +1920,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
restructuration des répertoires + duplication formats 21 > 22 (pour janvier-février avant maj fg/genrsa)
</commit_message>
<xml_diff>
--- a/formats/regpexpr/rg_curseurs.xlsx
+++ b/formats/regpexpr/rg_curseurs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/regpexpr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr_reshape/formats/regpexpr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B5F14D-32E0-0243-B542-1FC0AF6190F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB142C53-B5CD-A145-9889-C8AB526DD3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="27340" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="30">
   <si>
     <t>table</t>
   </si>
@@ -483,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="141" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="141" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2174,6 +2174,142 @@
         <v>23</v>
       </c>
       <c r="E99" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E102" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E103" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B104" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B105" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B106" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E106" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B107" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E107" s="1">
         <v>29</v>
       </c>
     </row>

</xml_diff>